<commit_message>
Update plots for problem 5 based on optimization
</commit_message>
<xml_diff>
--- a/hw4/file-swaps-durations.xlsx
+++ b/hw4/file-swaps-durations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\DM3PEPF00014772\EXCELCNV\8516aa3b-44c6-44d0-8d8a-8c2ecc430dcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45368E9F-4471-4111-A9CC-3B57895FB13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFFD79C-D67B-43A6-A2B8-E3CF0B199366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{8805CCD6-5D5D-4A15-8599-DA20BFBC0695}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -530,7 +536,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -624,7 +630,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Avg swap time for square matrix, ntrials = 5</a:t>
+              <a:t>Avg swap time for sqaure matrix, ntrials=5</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -733,37 +739,37 @@
             <c:numRef>
               <c:f>in!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.5353000000000007E-5</c:v>
+                  <c:v>-4.0599250065000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.860164E-4</c:v>
+                  <c:v>-3.7608081692000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7629740000000002E-4</c:v>
+                  <c:v>-3.4381730919</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.7555620000000001E-4</c:v>
+                  <c:v>-3.1510173116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5493157999999999E-3</c:v>
+                  <c:v>-2.8335545513999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1217492000000001E-3</c:v>
+                  <c:v>-2.5109881328000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6983538E-3</c:v>
+                  <c:v>-2.2044048759999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.54521478E-2</c:v>
+                  <c:v>-1.8382387171000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0978932399999999E-2</c:v>
+                  <c:v>-1.4895081672999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5111446000000003E-2</c:v>
+                  <c:v>-1.1984750653</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -771,7 +777,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D74E-43C3-9169-19A5F51D2E8F}"/>
+              <c16:uniqueId val="{00000003-D988-4B9A-A64F-4AF634F03C43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -844,37 +850,37 @@
             <c:numRef>
               <c:f>in!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.126126E-4</c:v>
+                  <c:v>-5.2232697671999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8059980000000001E-4</c:v>
+                  <c:v>-5.2068384708000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7596960000000002E-4</c:v>
+                  <c:v>-5.1931555211999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4562440000000003E-4</c:v>
+                  <c:v>-5.1801929354</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6140410000000001E-3</c:v>
+                  <c:v>-5.1258662211999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1049803999999999E-3</c:v>
+                  <c:v>-5.0950573613000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0081987999999996E-3</c:v>
+                  <c:v>-4.9652672931000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1993866400000001E-2</c:v>
+                  <c:v>-4.7996584824999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3924452999999998E-2</c:v>
+                  <c:v>-4.5780803374000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.7937400400000003E-2</c:v>
+                  <c:v>-4.3204285737000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -882,7 +888,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D74E-43C3-9169-19A5F51D2E8F}"/>
+              <c16:uniqueId val="{00000005-D988-4B9A-A64F-4AF634F03C43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -895,11 +901,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1081897479"/>
-        <c:axId val="1081899527"/>
+        <c:axId val="915065864"/>
+        <c:axId val="915076104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1081897479"/>
+        <c:axId val="915065864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1003,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1081899527"/>
+        <c:crossAx val="915076104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,9 +1011,8 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1081899527"/>
+        <c:axId val="915076104"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1047,7 +1052,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Swap time (log(s))</a:t>
+                  <a:t>log(s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1081,7 +1086,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1112,7 +1117,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1081897479"/>
+        <c:crossAx val="915065864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1752,23 +1757,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D59D84-2515-40A3-AF27-3C15F81F63CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBD3ED5-6806-A1D3-D24B-B483C4E288E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2089,7 +2094,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2114,10 +2119,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>9.5353000000000007E-5</v>
+        <v>-4.0599250065000003</v>
       </c>
       <c r="C2" s="1">
-        <v>1.126126E-4</v>
+        <v>-5.2232697671999997</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2125,10 +2130,10 @@
         <v>32</v>
       </c>
       <c r="B3" s="1">
-        <v>1.860164E-4</v>
+        <v>-3.7608081692000002</v>
       </c>
       <c r="C3" s="1">
-        <v>1.8059980000000001E-4</v>
+        <v>-5.2068384708000002</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2136,10 +2141,10 @@
         <v>64</v>
       </c>
       <c r="B4" s="1">
-        <v>3.7629740000000002E-4</v>
+        <v>-3.4381730919</v>
       </c>
       <c r="C4" s="1">
-        <v>3.7596960000000002E-4</v>
+        <v>-5.1931555211999996</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2147,10 +2152,10 @@
         <v>128</v>
       </c>
       <c r="B5" s="1">
-        <v>7.7555620000000001E-4</v>
+        <v>-3.1510173116</v>
       </c>
       <c r="C5" s="1">
-        <v>8.4562440000000003E-4</v>
+        <v>-5.1801929354</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2158,10 +2163,10 @@
         <v>256</v>
       </c>
       <c r="B6" s="1">
-        <v>1.5493157999999999E-3</v>
+        <v>-2.8335545513999998</v>
       </c>
       <c r="C6" s="1">
-        <v>1.6140410000000001E-3</v>
+        <v>-5.1258662211999999</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2169,10 +2174,10 @@
         <v>512</v>
       </c>
       <c r="B7" s="1">
-        <v>3.1217492000000001E-3</v>
+        <v>-2.5109881328000001</v>
       </c>
       <c r="C7" s="1">
-        <v>3.1049803999999999E-3</v>
+        <v>-5.0950573613000003</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2180,10 +2185,10 @@
         <v>1024</v>
       </c>
       <c r="B8" s="1">
-        <v>6.6983538E-3</v>
+        <v>-2.2044048759999999</v>
       </c>
       <c r="C8" s="1">
-        <v>6.0081987999999996E-3</v>
+        <v>-4.9652672931000001</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2191,10 +2196,10 @@
         <v>2048</v>
       </c>
       <c r="B9" s="1">
-        <v>1.54521478E-2</v>
+        <v>-1.8382387171000001</v>
       </c>
       <c r="C9" s="1">
-        <v>1.1993866400000001E-2</v>
+        <v>-4.7996584824999999</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2202,10 +2207,10 @@
         <v>4096</v>
       </c>
       <c r="B10" s="1">
-        <v>3.0978932399999999E-2</v>
+        <v>-1.4895081672999999</v>
       </c>
       <c r="C10" s="1">
-        <v>2.3924452999999998E-2</v>
+        <v>-4.5780803374000003</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2213,10 +2218,10 @@
         <v>8192</v>
       </c>
       <c r="B11" s="1">
-        <v>6.5111446000000003E-2</v>
+        <v>-1.1984750653</v>
       </c>
       <c r="C11" s="1">
-        <v>4.7937400400000003E-2</v>
+        <v>-4.3204285737000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>